<commit_message>
milestone all field test
</commit_message>
<xml_diff>
--- a/src/test/resources/manual_TestCases/RunnerTestCaseMasterSheet.xlsx
+++ b/src/test/resources/manual_TestCases/RunnerTestCaseMasterSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91902\IdeaProjects\Selenium_E2E_Automation_framework\src\test\resources\manual_TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23A532B-D3A2-412F-B48C-7EB6DF4D6F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE00D6E7-4880-4B7D-9D64-C7B508B4EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>TEST_CASE_ID</t>
   </si>
@@ -184,6 +184,32 @@
     <t>Name: Adi
 Code: 245
 Workflow: Booking/Custome-Booking/CONSOLIDATION/ORDER/QUOTE/SHIPMENT/ACCOUNT_PAYABLE</t>
+  </si>
+  <si>
+    <t>TC_MILESTONE_02</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify create new milestone feature is working
+with all fields to be used. </t>
+  </si>
+  <si>
+    <t>All datas are filled and CREATE button should enable</t>
+  </si>
+  <si>
+    <t>5. Fill all fields present in create new milestone and for each workflow type add different datas while creating milestone. And for check ACTIVE is always ticked rest two 
+fill alternately and both while creating milestone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name: Adi
+Code: 245
+Workflow: Booking/Custome-Booking/CONSOLIDATION/ORDER/QUOTE/SHIPMENT/ACCOUNT_PAYABLE
+Milestone description:
+new milestone.
+Show on milestone
+</t>
   </si>
 </sst>
 </file>
@@ -338,45 +364,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,14 +406,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,13 +754,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -751,14 +779,14 @@
         <v>17</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="17"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
@@ -773,12 +801,12 @@
         <v>21</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="13"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
@@ -793,12 +821,12 @@
         <v>24</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="13"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
         <v>26</v>
@@ -813,12 +841,12 @@
         <v>28</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="13"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="17"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -831,7 +859,7 @@
         <v>31</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="13"/>
+      <c r="J6" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -846,10 +874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD0B06F-D086-4938-9AA0-C3AEEEA0202B}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,163 +886,276 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="52.140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" style="11" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="13"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="1" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="19" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="13"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="11" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="13"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="13"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="19" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+    </row>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="26"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="26"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>